<commit_message>
new schemas of Multipulse_feature
</commit_message>
<xml_diff>
--- a/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
+++ b/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/letrung/Documents/MATLAB/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AE0B8E-D957-2844-AE40-FA8474B8D6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1737BFC-5AFA-F94B-9CC0-F03A08B4E166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12660" yWindow="980" windowWidth="27640" windowHeight="15580" xr2:uid="{A92255C9-FE15-A842-B8F3-999E40995B9A}"/>
+    <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15580" xr2:uid="{A92255C9-FE15-A842-B8F3-999E40995B9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Field</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>uint16</t>
+  </si>
+  <si>
+    <t>features</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAC3773-BB46-8342-89C6-DFE915895E05}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,6 +792,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix field name Featureextract
</commit_message>
<xml_diff>
--- a/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
+++ b/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/letrung/Documents/MATLAB/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1737BFC-5AFA-F94B-9CC0-F03A08B4E166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57309CAC-D402-7C41-9E18-6177541C8966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15580" xr2:uid="{A92255C9-FE15-A842-B8F3-999E40995B9A}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix things in sln results table
</commit_message>
<xml_diff>
--- a/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
+++ b/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/letrung/Documents/MATLAB/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F222C52B-0448-134F-8DE5-304F1F7CF9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C07C831-AA07-0744-8062-6723B9073B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13900" yWindow="640" windowWidth="27640" windowHeight="15580" xr2:uid="{A92255C9-FE15-A842-B8F3-999E40995B9A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{A92255C9-FE15-A842-B8F3-999E40995B9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>Field</t>
   </si>
@@ -188,96 +188,33 @@
     <t>resistance</t>
   </si>
   <si>
-    <t>resistance_Rsquared</t>
-  </si>
-  <si>
-    <t>membrane resistance (MOhm) - array from each trial</t>
-  </si>
-  <si>
-    <t>GOF adjusted R square of resistance calculation - from each trial</t>
-  </si>
-  <si>
     <t>tau</t>
   </si>
   <si>
-    <t>membrane time constant (ms) - from each trial</t>
-  </si>
-  <si>
     <t>capacitance</t>
   </si>
   <si>
-    <t>membrane capacitance (pF) - from each trial</t>
-  </si>
-  <si>
     <t>sag</t>
   </si>
   <si>
-    <t>coefficient of sag amplitude in hyperpolarizing epochs - from each trial</t>
-  </si>
-  <si>
     <t>spontaneous_firing_rate</t>
   </si>
   <si>
-    <t>spontaneous firing rate at rest (Hz) - from each trial</t>
-  </si>
-  <si>
-    <t>V_threshold</t>
-  </si>
-  <si>
-    <t>AP threshold voltage (20% of max dV/dt) - from each trial (mV)</t>
-  </si>
-  <si>
     <t>half_width_time</t>
   </si>
   <si>
-    <t>first_AP_peak_amplitude</t>
-  </si>
-  <si>
-    <t>First AP peak amplitude(mV)</t>
-  </si>
-  <si>
-    <t>first_AP_peak_time</t>
-  </si>
-  <si>
-    <t>Half width time of first AP (ms) - from each trial (mV)</t>
-  </si>
-  <si>
-    <t>first_AP_trough_amplitude</t>
-  </si>
-  <si>
-    <t>first_AP_trough_time</t>
-  </si>
-  <si>
-    <t>First AP trough amplitude(mV)</t>
-  </si>
-  <si>
     <t>max_number_of_spike</t>
   </si>
   <si>
-    <t xml:space="preserve">Max number of spikes from any depolarization epochs </t>
-  </si>
-  <si>
-    <t>First AP peak location (ms)</t>
-  </si>
-  <si>
-    <t>First AP trough location (ms)</t>
-  </si>
-  <si>
     <t>current_max_number_of_spike</t>
   </si>
   <si>
-    <t>Depolarization current at which max number of spikes is achieved</t>
-  </si>
-  <si>
     <t>max_latency_of_spike</t>
   </si>
   <si>
     <t>max_adaptation_index</t>
   </si>
   <si>
-    <t>max_ISI_CV</t>
-  </si>
-  <si>
     <t>first_current_level_to_block</t>
   </si>
   <si>
@@ -287,12 +224,6 @@
     <t>half_max_spike_current</t>
   </si>
   <si>
-    <t>Nspike_max_vs_last_epoch_ratio</t>
-  </si>
-  <si>
-    <t>max_AHP_after_depol_injection</t>
-  </si>
-  <si>
     <t>max_63_percent_decay_time</t>
   </si>
   <si>
@@ -305,40 +236,31 @@
     <t>spontenous_spike_amplitude_cv</t>
   </si>
   <si>
-    <t>Max latency to first spike (ms)</t>
-  </si>
-  <si>
-    <t>Max adaptation index through all depolarization epochs of eacg trial</t>
-  </si>
-  <si>
-    <t>Max ISI CV of depol epochs from each trial</t>
-  </si>
-  <si>
-    <t>First current (pA) to get depol block</t>
-  </si>
-  <si>
-    <t>Max AP slope of first AP (V/s)</t>
-  </si>
-  <si>
-    <t>Half max of spike numbers (increasing side only on f-I curve)</t>
-  </si>
-  <si>
-    <t>Current at which half max of spike number on f-I curve</t>
-  </si>
-  <si>
-    <t>Ratio of max number of spike over spikes from max depol epoch</t>
-  </si>
-  <si>
-    <t>Max AHP after depol (to a find windows of 10ms) (mV)</t>
-  </si>
-  <si>
-    <t>Max time during depol current inj that AP decay 1/e (ms)</t>
-  </si>
-  <si>
-    <t>Min time during depol current inj that AP decay 1/e (ms)</t>
-  </si>
-  <si>
-    <t>CV of all spontaneous spikes amplitude</t>
+    <t>nspike_ratio</t>
+  </si>
+  <si>
+    <t>v_threshold</t>
+  </si>
+  <si>
+    <t>first_ap_peak_amplitude</t>
+  </si>
+  <si>
+    <t>first_ap_peak_time</t>
+  </si>
+  <si>
+    <t>first_ap_trough_amplitude</t>
+  </si>
+  <si>
+    <t>first_ap_trough_time</t>
+  </si>
+  <si>
+    <t>max_isi_cv</t>
+  </si>
+  <si>
+    <t>max_ahp_after_depol_injection</t>
+  </si>
+  <si>
+    <t>resistance_rsquared</t>
   </si>
 </sst>
 </file>
@@ -692,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAC3773-BB46-8342-89C6-DFE915895E05}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,283 +874,205 @@
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>84</v>
-      </c>
       <c r="B45" t="s">
         <v>4</v>
       </c>
-      <c r="C45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
-      <c r="C46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
-      <c r="C47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
-      </c>
-      <c r="C48" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel file template
</commit_message>
<xml_diff>
--- a/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
+++ b/result_table_templates/MultiPulse_varyCurrent_FeatureExtract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/letrung/Documents/MATLAB/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E4A5E5-EF8B-6540-80FA-34F612FD9112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D7952F-248C-F44A-B939-AE68DF7266C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15660" yWindow="2260" windowWidth="28800" windowHeight="16080" xr2:uid="{A92255C9-FE15-A842-B8F3-999E40995B9A}"/>
+    <workbookView xWindow="14340" yWindow="1300" windowWidth="28800" windowHeight="16080" xr2:uid="{A92255C9-FE15-A842-B8F3-999E40995B9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
   <si>
     <t>Field</t>
   </si>
@@ -261,6 +261,84 @@
   </si>
   <si>
     <t>resistance_rsquared</t>
+  </si>
+  <si>
+    <t>membrane resistance (mohm)  array from each trial</t>
+  </si>
+  <si>
+    <t>gof adjusted r square of resistance calculation  from each trial</t>
+  </si>
+  <si>
+    <t>membrane time constant (ms)  from each trial</t>
+  </si>
+  <si>
+    <t>membrane capacitance (pf)  from each trial</t>
+  </si>
+  <si>
+    <t>coefficient of sag amplitude in hyperpolarizing eps  from each trial</t>
+  </si>
+  <si>
+    <t>spontaneous firing rate at rest (hz)  from each trial</t>
+  </si>
+  <si>
+    <t>half width time of first ap (ms)  from each trial (mv)</t>
+  </si>
+  <si>
+    <t>first ap peak amplitude(mv)</t>
+  </si>
+  <si>
+    <t>first ap peak location (ms)</t>
+  </si>
+  <si>
+    <t>first ap trough amplitude(mv)</t>
+  </si>
+  <si>
+    <t>first ap trough location (ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max number of spikes from any depolarization eps </t>
+  </si>
+  <si>
+    <t>depolarization current at which max number of spikes is achieved</t>
+  </si>
+  <si>
+    <t>max latency to first spike (ms)</t>
+  </si>
+  <si>
+    <t>max adaptation index through all depolarization eps of eacg trial</t>
+  </si>
+  <si>
+    <t>max isi cv of depol eps from each trial</t>
+  </si>
+  <si>
+    <t>first current (pa) to get depol block</t>
+  </si>
+  <si>
+    <t>max ap slope of first ap (vs)</t>
+  </si>
+  <si>
+    <t>half max of spike numbers (increasing side only on fi curve)</t>
+  </si>
+  <si>
+    <t>current at which half max of spike number on fi curve</t>
+  </si>
+  <si>
+    <t>max ahp after depol (to a find windows of 10ms) (mv)</t>
+  </si>
+  <si>
+    <t>max time during depol current inj that ap decay 1e (ms)</t>
+  </si>
+  <si>
+    <t>min time during depol current inj that ap decay 1e (ms)</t>
+  </si>
+  <si>
+    <t>cv of all spontaneous spikes amplitude</t>
+  </si>
+  <si>
+    <t>ap threshold voltage (20 percent of max dvdt)  from each trial (mv)</t>
+  </si>
+  <si>
+    <t>max number of spike over last depolarizing epoch number of spikes</t>
   </si>
 </sst>
 </file>
@@ -614,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAC3773-BB46-8342-89C6-DFE915895E05}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,6 +952,9 @@
       <c r="B23" t="s">
         <v>4</v>
       </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -882,6 +963,9 @@
       <c r="B24" t="s">
         <v>4</v>
       </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -890,6 +974,9 @@
       <c r="B25" t="s">
         <v>4</v>
       </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -898,6 +985,9 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -906,6 +996,9 @@
       <c r="B27" t="s">
         <v>4</v>
       </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -914,6 +1007,9 @@
       <c r="B28" t="s">
         <v>4</v>
       </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -922,6 +1018,9 @@
       <c r="B29" t="s">
         <v>4</v>
       </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -930,6 +1029,9 @@
       <c r="B30" t="s">
         <v>4</v>
       </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -938,6 +1040,9 @@
       <c r="B31" t="s">
         <v>4</v>
       </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -946,133 +1051,184 @@
       <c r="B32" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>55</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>57</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>59</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>64</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>60</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>61</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>66</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>63</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>65</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>